<commit_message>
Efficient max field calcs, new sections
</commit_message>
<xml_diff>
--- a/XC-comparisons/32E-DAT_comparison.xlsx
+++ b/XC-comparisons/32E-DAT_comparison.xlsx
@@ -731,7 +731,7 @@
         <v>-290</v>
       </c>
       <c r="B12">
-        <v>-0.00100000000000477</v>
+        <v>-2.8421709430404e-14</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2036,7 +2036,7 @@
         <v>-245</v>
       </c>
       <c r="B57">
-        <v>-0.000999999999976353</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2210,7 +2210,7 @@
         <v>-239</v>
       </c>
       <c r="B63">
-        <v>-0.00100000000009004</v>
+        <v>-1.13686837721616e-13</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2268,7 +2268,7 @@
         <v>-237</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.00100000000009004</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2819,7 +2819,7 @@
         <v>-218</v>
       </c>
       <c r="B84">
-        <v>-0.000999999999976353</v>
+        <v>0</v>
       </c>
       <c r="C84">
         <v>1.13686837721616e-13</v>
@@ -4037,7 +4037,7 @@
         <v>-176</v>
       </c>
       <c r="B126">
-        <v>-0.000999999999976353</v>
+        <v>1.13686837721616e-13</v>
       </c>
       <c r="C126">
         <v>-1.13686837721616e-13</v>
@@ -4965,7 +4965,7 @@
         <v>-144</v>
       </c>
       <c r="B158">
-        <v>-0.0010000000000332</v>
+        <v>-5.6843418860808e-14</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -5893,7 +5893,7 @@
         <v>-112</v>
       </c>
       <c r="B190">
-        <v>-0.000999999999976353</v>
+        <v>0</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -6531,7 +6531,7 @@
         <v>-90</v>
       </c>
       <c r="B212">
-        <v>-1.13686837721616e-13</v>
+        <v>0.000999999999976353</v>
       </c>
       <c r="C212">
         <v>1.13686837721616e-13</v>
@@ -7343,7 +7343,7 @@
         <v>-62</v>
       </c>
       <c r="B240">
-        <v>-0.00100000000009004</v>
+        <v>-1.13686837721616e-13</v>
       </c>
       <c r="C240">
         <v>0</v>
@@ -8619,7 +8619,7 @@
         <v>-18</v>
       </c>
       <c r="B284">
-        <v>0</v>
+        <v>0.000999999999976353</v>
       </c>
       <c r="C284">
         <v>0</v>
@@ -8793,7 +8793,7 @@
         <v>-12</v>
       </c>
       <c r="B290">
-        <v>-0.000999999999976353</v>
+        <v>0</v>
       </c>
       <c r="C290">
         <v>0</v>
@@ -9054,7 +9054,7 @@
         <v>-3</v>
       </c>
       <c r="B299">
-        <v>0</v>
+        <v>0.000999999999976353</v>
       </c>
       <c r="C299">
         <v>0</v>
@@ -9199,7 +9199,7 @@
         <v>2</v>
       </c>
       <c r="B304">
-        <v>-0.0010000000000332</v>
+        <v>0</v>
       </c>
       <c r="C304">
         <v>0</v>
@@ -12418,7 +12418,7 @@
         <v>113</v>
       </c>
       <c r="B415">
-        <v>-5.6843418860808e-14</v>
+        <v>0.000999999999976353</v>
       </c>
       <c r="C415">
         <v>0.00099999999991951</v>
@@ -12476,7 +12476,7 @@
         <v>115</v>
       </c>
       <c r="B417">
-        <v>0</v>
+        <v>0.000999999999976353</v>
       </c>
       <c r="C417">
         <v>-5.6843418860808e-14</v>
@@ -13433,7 +13433,7 @@
         <v>148</v>
       </c>
       <c r="B450">
-        <v>-0.000999999999976353</v>
+        <v>1.13686837721616e-13</v>
       </c>
       <c r="C450">
         <v>0</v>
@@ -13520,7 +13520,7 @@
         <v>151</v>
       </c>
       <c r="B453">
-        <v>-0.000999999999976353</v>
+        <v>0</v>
       </c>
       <c r="C453">
         <v>0</v>
@@ -13868,7 +13868,7 @@
         <v>163</v>
       </c>
       <c r="B465">
-        <v>0</v>
+        <v>0.000999999999976353</v>
       </c>
       <c r="C465">
         <v>0</v>
@@ -35673,7 +35673,7 @@
         <v>-290</v>
       </c>
       <c r="B12">
-        <v>163.58</v>
+        <v>163.581</v>
       </c>
       <c r="C12">
         <v>163.733</v>
@@ -36978,7 +36978,7 @@
         <v>-245</v>
       </c>
       <c r="B57">
-        <v>639.678</v>
+        <v>639.679</v>
       </c>
       <c r="C57">
         <v>646.702</v>
@@ -37152,7 +37152,7 @@
         <v>-239</v>
       </c>
       <c r="B63">
-        <v>763.515</v>
+        <v>763.516</v>
       </c>
       <c r="C63">
         <v>776.32</v>
@@ -37210,7 +37210,7 @@
         <v>-237</v>
       </c>
       <c r="B65">
-        <v>798.43</v>
+        <v>798.431</v>
       </c>
       <c r="C65">
         <v>813.945</v>
@@ -37761,7 +37761,7 @@
         <v>-218</v>
       </c>
       <c r="B84">
-        <v>830.945</v>
+        <v>830.946</v>
       </c>
       <c r="C84">
         <v>906.667</v>
@@ -38979,7 +38979,7 @@
         <v>-176</v>
       </c>
       <c r="B126">
-        <v>832.521</v>
+        <v>832.522</v>
       </c>
       <c r="C126">
         <v>880.616</v>
@@ -39907,7 +39907,7 @@
         <v>-144</v>
       </c>
       <c r="B158">
-        <v>445.752</v>
+        <v>445.753</v>
       </c>
       <c r="C158">
         <v>457.05</v>
@@ -40835,7 +40835,7 @@
         <v>-112</v>
       </c>
       <c r="B190">
-        <v>390.744</v>
+        <v>390.745</v>
       </c>
       <c r="C190">
         <v>401.092</v>
@@ -41473,7 +41473,7 @@
         <v>-90</v>
       </c>
       <c r="B212">
-        <v>712.406</v>
+        <v>712.407</v>
       </c>
       <c r="C212">
         <v>732.519</v>
@@ -42285,7 +42285,7 @@
         <v>-62</v>
       </c>
       <c r="B240">
-        <v>791.837</v>
+        <v>791.838</v>
       </c>
       <c r="C240">
         <v>904.347</v>
@@ -43561,7 +43561,7 @@
         <v>-18</v>
       </c>
       <c r="B284">
-        <v>851.212</v>
+        <v>851.213</v>
       </c>
       <c r="C284">
         <v>874.368</v>
@@ -43735,7 +43735,7 @@
         <v>-12</v>
       </c>
       <c r="B290">
-        <v>772.328</v>
+        <v>772.329</v>
       </c>
       <c r="C290">
         <v>785.319</v>
@@ -43996,7 +43996,7 @@
         <v>-3</v>
       </c>
       <c r="B299">
-        <v>584.335</v>
+        <v>584.336</v>
       </c>
       <c r="C299">
         <v>589.18</v>
@@ -44141,7 +44141,7 @@
         <v>2</v>
       </c>
       <c r="B304">
-        <v>484.96</v>
+        <v>484.961</v>
       </c>
       <c r="C304">
         <v>487.642</v>
@@ -47360,7 +47360,7 @@
         <v>113</v>
       </c>
       <c r="B415">
-        <v>340.198</v>
+        <v>340.199</v>
       </c>
       <c r="C415">
         <v>362.929</v>
@@ -47418,7 +47418,7 @@
         <v>115</v>
       </c>
       <c r="B417">
-        <v>375.309</v>
+        <v>375.31</v>
       </c>
       <c r="C417">
         <v>397.133</v>
@@ -48375,7 +48375,7 @@
         <v>148</v>
       </c>
       <c r="B450">
-        <v>700.228</v>
+        <v>700.229</v>
       </c>
       <c r="C450">
         <v>701.179</v>
@@ -48462,7 +48462,7 @@
         <v>151</v>
       </c>
       <c r="B453">
-        <v>712.364</v>
+        <v>712.365</v>
       </c>
       <c r="C453">
         <v>713.253</v>
@@ -48810,7 +48810,7 @@
         <v>163</v>
       </c>
       <c r="B465">
-        <v>811.255</v>
+        <v>811.256</v>
       </c>
       <c r="C465">
         <v>815.187</v>
@@ -53144,7 +53144,7 @@
         <v>-290</v>
       </c>
       <c r="B12">
-        <v>-0.000611321677469602</v>
+        <v>-1.73747008701524e-14</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -54449,7 +54449,7 @@
         <v>-245</v>
       </c>
       <c r="B57">
-        <v>-0.00015632865284977</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -54623,7 +54623,7 @@
         <v>-239</v>
       </c>
       <c r="B63">
-        <v>-0.000130973196347163</v>
+        <v>-1.48899090158708e-14</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -54681,7 +54681,7 @@
         <v>-237</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.000125245638018819</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -55232,7 +55232,7 @@
         <v>-218</v>
       </c>
       <c r="B84">
-        <v>-0.000120344908504938</v>
+        <v>0</v>
       </c>
       <c r="C84">
         <v>1.25389848446691e-14</v>
@@ -56450,7 +56450,7 @@
         <v>-176</v>
       </c>
       <c r="B126">
-        <v>-0.000120117090136628</v>
+        <v>1.365571573143e-14</v>
       </c>
       <c r="C126">
         <v>-1.29099218866811e-14</v>
@@ -57378,7 +57378,7 @@
         <v>-144</v>
       </c>
       <c r="B158">
-        <v>-0.000224339991751736</v>
+        <v>-1.27522235096136e-14</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -58306,7 +58306,7 @@
         <v>-112</v>
       </c>
       <c r="B190">
-        <v>-0.000255922035904928</v>
+        <v>0</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -58944,7 +58944,7 @@
         <v>-90</v>
       </c>
       <c r="B212">
-        <v>-1.59581527558185e-14</v>
+        <v>0.000140369199064068</v>
       </c>
       <c r="C212">
         <v>1.55199848361088e-14</v>
@@ -59756,7 +59756,7 @@
         <v>-62</v>
       </c>
       <c r="B240">
-        <v>-0.000126288617491989</v>
+        <v>-1.43573354299258e-14</v>
       </c>
       <c r="C240">
         <v>0</v>
@@ -61032,7 +61032,7 @@
         <v>-18</v>
       </c>
       <c r="B284">
-        <v>0</v>
+        <v>0.000117479408793845</v>
       </c>
       <c r="C284">
         <v>0</v>
@@ -61206,7 +61206,7 @@
         <v>-12</v>
       </c>
       <c r="B290">
-        <v>-0.000129478667091748</v>
+        <v>0</v>
       </c>
       <c r="C290">
         <v>0</v>
@@ -61467,7 +61467,7 @@
         <v>-3</v>
       </c>
       <c r="B299">
-        <v>0</v>
+        <v>0.000171134415811511</v>
       </c>
       <c r="C299">
         <v>0</v>
@@ -61612,7 +61612,7 @@
         <v>2</v>
       </c>
       <c r="B304">
-        <v>-0.000206202573414961</v>
+        <v>0</v>
       </c>
       <c r="C304">
         <v>0</v>
@@ -64831,7 +64831,7 @@
         <v>113</v>
       </c>
       <c r="B415">
-        <v>-1.67089221161818e-14</v>
+        <v>0.000293945602419864</v>
       </c>
       <c r="C415">
         <v>0.000275535986355323</v>
@@ -64889,7 +64889,7 @@
         <v>115</v>
       </c>
       <c r="B417">
-        <v>0</v>
+        <v>0.000266446404299473</v>
       </c>
       <c r="C417">
         <v>-1.43134463418573e-14</v>
@@ -65846,7 +65846,7 @@
         <v>148</v>
       </c>
       <c r="B450">
-        <v>-0.000142810627392271</v>
+        <v>1.62356654353956e-14</v>
       </c>
       <c r="C450">
         <v>0</v>
@@ -65933,7 +65933,7 @@
         <v>151</v>
       </c>
       <c r="B453">
-        <v>-0.000140377672085669</v>
+        <v>0</v>
       </c>
       <c r="C453">
         <v>0</v>
@@ -66281,7 +66281,7 @@
         <v>163</v>
       </c>
       <c r="B465">
-        <v>0</v>
+        <v>0.000123265652269611</v>
       </c>
       <c r="C465">
         <v>0</v>

</xml_diff>